<commit_message>
Changed Inpatient and Outpatient
</commit_message>
<xml_diff>
--- a/QMRProject/TestData/MasterData.xlsx
+++ b/QMRProject/TestData/MasterData.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="106">
   <si>
     <t>S.No</t>
   </si>
@@ -317,6 +317,33 @@
   </si>
   <si>
     <t>2021_08_03_03_17_36</t>
+  </si>
+  <si>
+    <t>2021_08_05_12_29_32</t>
+  </si>
+  <si>
+    <t>2021_08_05_12_44_46</t>
+  </si>
+  <si>
+    <t>2021_08_05_12_48_34</t>
+  </si>
+  <si>
+    <t>2021_08_05_12_52_21</t>
+  </si>
+  <si>
+    <t>2021_08_05_12_59_29</t>
+  </si>
+  <si>
+    <t>2021_08_05_01_02_39</t>
+  </si>
+  <si>
+    <t>2021_08_05_01_08_18</t>
+  </si>
+  <si>
+    <t>2021_08_05_01_25_55</t>
+  </si>
+  <si>
+    <t>2021_08_05_01_31_40</t>
   </si>
 </sst>
 </file>
@@ -778,7 +805,7 @@
         <v>86</v>
       </c>
       <c r="G2" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
     </row>
     <row r="3" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">

</xml_diff>